<commit_message>
added ability to filter by province
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,13 +418,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Alphen aan den Rijn</v>
+        <v>Heerlen</v>
       </c>
       <c r="B2" t="str">
-        <v>NS station</v>
+        <v>NS Centraal (bushaltes)</v>
       </c>
       <c r="C2" t="str">
-        <v>€ 38,50</v>
+        <v>€ 43,00</v>
       </c>
       <c r="D2" t="str">
         <v>1 oktober</v>
@@ -432,13 +432,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Delft</v>
+        <v>Kerkrade</v>
       </c>
       <c r="B3" t="str">
-        <v>Hampshire hotel Delft Centre</v>
+        <v>NS Centrum</v>
       </c>
       <c r="C3" t="str">
-        <v>€ 40,50</v>
+        <v>€ 43,50</v>
       </c>
       <c r="D3" t="str">
         <v>1 oktober</v>
@@ -446,13 +446,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Den Haag</v>
+        <v>Maastricht</v>
       </c>
       <c r="B4" t="str">
-        <v>Busplaatsen thv. Academie van Beeldende Kunsten</v>
+        <v>parkeerplaats Geusselt Maastricht</v>
       </c>
       <c r="C4" t="str">
-        <v>€ 40,50</v>
+        <v>€ 43,00</v>
       </c>
       <c r="D4" t="str">
         <v>1 oktober</v>
@@ -460,13 +460,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Dordrecht</v>
+        <v>Roermond</v>
       </c>
       <c r="B5" t="str">
-        <v>NS Centraal (Voorzijde - bij de stadsbussen)</v>
+        <v>NS station</v>
       </c>
       <c r="C5" t="str">
-        <v>€ 38,50</v>
+        <v>€ 39,50</v>
       </c>
       <c r="D5" t="str">
         <v>1 oktober</v>
@@ -474,13 +474,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Gorinchem</v>
+        <v>Venlo</v>
       </c>
       <c r="B6" t="str">
         <v>NS station</v>
       </c>
       <c r="C6" t="str">
-        <v>€ 35,00</v>
+        <v>€ 36,50</v>
       </c>
       <c r="D6" t="str">
         <v>1 oktober</v>
@@ -488,13 +488,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Gouda</v>
+        <v>Well</v>
       </c>
       <c r="B7" t="str">
-        <v>Station (Achterzijde t.h.v. Cinema Gouda)</v>
+        <v>BP Tankstation Moleneind</v>
       </c>
       <c r="C7" t="str">
-        <v>€ 38,00</v>
+        <v>€ 33,50</v>
       </c>
       <c r="D7" t="str">
         <v>1 oktober</v>
@@ -502,161 +502,21 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Hillegom</v>
+        <v>Wellerlooi</v>
       </c>
       <c r="B8" t="str">
-        <v>NS station</v>
+        <v>Bushalte Catharinastraat</v>
       </c>
       <c r="C8" t="str">
-        <v>€ 40,50</v>
+        <v>€ 34,00</v>
       </c>
       <c r="D8" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Katwijk</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Parkeerplaats vv Katwijk</v>
-      </c>
-      <c r="C9" t="str">
-        <v>€ 40,50</v>
-      </c>
-      <c r="D9" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>Krimpen aan de Lek</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Bushalte De Viersprong (N210, rotonde)</v>
-      </c>
-      <c r="C10" t="str">
-        <v>€ 39,00</v>
-      </c>
-      <c r="D10" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>Krimpen aan den IJssel</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Zwembad De Lansingh</v>
-      </c>
-      <c r="C11" t="str">
-        <v>€ 40,00</v>
-      </c>
-      <c r="D11" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>Leiden</v>
-      </c>
-      <c r="B12" t="str">
-        <v>NS Lammenschans</v>
-      </c>
-      <c r="C12" t="str">
-        <v>€ 39,50</v>
-      </c>
-      <c r="D12" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>Nootdorp</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Metrostation Nootdorp P+R (Industriezijde)</v>
-      </c>
-      <c r="C13" t="str">
-        <v>€ 40,00</v>
-      </c>
-      <c r="D13" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>Rotterdam</v>
-      </c>
-      <c r="B14" t="str">
-        <v>NS Centraal (Kiss &amp; Ride) - Conradstraat</v>
-      </c>
-      <c r="C14" t="str">
-        <v>€ 40,00</v>
-      </c>
-      <c r="D14" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>Rotterdam</v>
-      </c>
-      <c r="B15" t="str">
-        <v>Metrostation Slinge (bushalte aan Zuiderparkweg)</v>
-      </c>
-      <c r="C15" t="str">
-        <v>€ 40,00</v>
-      </c>
-      <c r="D15" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="str">
-        <v>Schiedam</v>
-      </c>
-      <c r="B16" t="str">
-        <v>Sporthal Margriet</v>
-      </c>
-      <c r="C16" t="str">
-        <v>€ 41,00</v>
-      </c>
-      <c r="D16" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="str">
-        <v>Spijkenisse</v>
-      </c>
-      <c r="B17" t="str">
-        <v>Kinepolis</v>
-      </c>
-      <c r="C17" t="str">
-        <v>€ 40,50</v>
-      </c>
-      <c r="D17" t="str">
-        <v>1 oktober</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>Zoetermeer</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Centrum West Bushalte</v>
-      </c>
-      <c r="C18" t="str">
-        <v>€ 39,50</v>
-      </c>
-      <c r="D18" t="str">
         <v>1 oktober</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
now combines all data of all provinces together
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,13 +418,13 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Heerlen</v>
+        <v>Groningen</v>
       </c>
       <c r="B2" t="str">
-        <v>NS Centraal (bushaltes)</v>
+        <v>NS Centraal (Flixbus halte)</v>
       </c>
       <c r="C2" t="str">
-        <v>€ 43,00</v>
+        <v>€ 44,00</v>
       </c>
       <c r="D2" t="str">
         <v>1 oktober</v>
@@ -432,13 +432,13 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Kerkrade</v>
+        <v>Winschoten</v>
       </c>
       <c r="B3" t="str">
-        <v>NS Centrum</v>
+        <v>NS station (Bushaltes)</v>
       </c>
       <c r="C3" t="str">
-        <v>€ 43,50</v>
+        <v>€ 45,00</v>
       </c>
       <c r="D3" t="str">
         <v>1 oktober</v>
@@ -446,13 +446,13 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Maastricht</v>
+        <v>Damwâld</v>
       </c>
       <c r="B4" t="str">
-        <v>parkeerplaats Geusselt Maastricht</v>
+        <v>Birwa Damwald</v>
       </c>
       <c r="C4" t="str">
-        <v>€ 43,00</v>
+        <v>€ 45,00</v>
       </c>
       <c r="D4" t="str">
         <v>1 oktober</v>
@@ -460,13 +460,13 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Roermond</v>
+        <v>Heerenveen</v>
       </c>
       <c r="B5" t="str">
-        <v>NS station</v>
+        <v>McDonalds Heerenveen</v>
       </c>
       <c r="C5" t="str">
-        <v>€ 39,50</v>
+        <v>€ 41,50</v>
       </c>
       <c r="D5" t="str">
         <v>1 oktober</v>
@@ -474,13 +474,13 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Venlo</v>
+        <v>Leeuwarden</v>
       </c>
       <c r="B6" t="str">
         <v>NS station</v>
       </c>
       <c r="C6" t="str">
-        <v>€ 36,50</v>
+        <v>€ 43,50</v>
       </c>
       <c r="D6" t="str">
         <v>1 oktober</v>
@@ -488,13 +488,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>Well</v>
+        <v>Leeuwarden</v>
       </c>
       <c r="B7" t="str">
-        <v>BP Tankstation Moleneind</v>
+        <v>uitstapbushalte busstation, stationsplein (Perron K)</v>
       </c>
       <c r="C7" t="str">
-        <v>€ 33,50</v>
+        <v>€ 43,50</v>
       </c>
       <c r="D7" t="str">
         <v>1 oktober</v>
@@ -502,21 +502,1197 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
+        <v>Assen</v>
+      </c>
+      <c r="B8" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C8" t="str">
+        <v>€ 42,50</v>
+      </c>
+      <c r="D8" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Emmen</v>
+      </c>
+      <c r="B9" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C9" t="str">
+        <v>€ 42,50</v>
+      </c>
+      <c r="D9" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Meppel</v>
+      </c>
+      <c r="B10" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C10" t="str">
+        <v>€ 38,00</v>
+      </c>
+      <c r="D10" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Meppel</v>
+      </c>
+      <c r="B11" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C11" t="str">
+        <v>€ 38,00</v>
+      </c>
+      <c r="D11" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Almelo</v>
+      </c>
+      <c r="B12" t="str">
+        <v>NS centraal (achterzijde parkeerplaats)</v>
+      </c>
+      <c r="C12" t="str">
+        <v>€ 36,50</v>
+      </c>
+      <c r="D12" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Almelo</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Tourbushalte (thv ingang java toren)</v>
+      </c>
+      <c r="C13" t="str">
+        <v>€ 36,50</v>
+      </c>
+      <c r="D13" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Dedemsvaart</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Bushalte Zwiersstraat thv Skatebaan</v>
+      </c>
+      <c r="C14" t="str">
+        <v>€ 38,50</v>
+      </c>
+      <c r="D14" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Enschede</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Het Diekman</v>
+      </c>
+      <c r="C15" t="str">
+        <v>€ 38,00</v>
+      </c>
+      <c r="D15" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Hardenberg</v>
+      </c>
+      <c r="B16" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C16" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D16" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Hengelo</v>
+      </c>
+      <c r="B17" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C17" t="str">
+        <v>€ 37,00</v>
+      </c>
+      <c r="D17" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Hengelo</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Schouwburg Hengelo</v>
+      </c>
+      <c r="C18" t="str">
+        <v>€ 37,00</v>
+      </c>
+      <c r="D18" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Rijssen</v>
+      </c>
+      <c r="B19" t="str">
+        <v>P+R Rijssen (Achterzijde NS Station Rijssen)</v>
+      </c>
+      <c r="C19" t="str">
+        <v>€ 34,50</v>
+      </c>
+      <c r="D19" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>Zwolle</v>
+      </c>
+      <c r="B20" t="str">
+        <v>NS Centraal (achterzijde)</v>
+      </c>
+      <c r="C20" t="str">
+        <v>€ 34,00</v>
+      </c>
+      <c r="D20" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>Almere</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Touringcar parking Almere Centrum (T.H.V. Gemeentehuis)</v>
+      </c>
+      <c r="C21" t="str">
+        <v>€ 37,00</v>
+      </c>
+      <c r="D21" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>Apeldoorn</v>
+      </c>
+      <c r="B22" t="str">
+        <v>Restaurant Orange (achterzijde)</v>
+      </c>
+      <c r="C22" t="str">
+        <v>€ 28,50</v>
+      </c>
+      <c r="D22" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>Barneveld</v>
+      </c>
+      <c r="B23" t="str">
+        <v>NS Centrum</v>
+      </c>
+      <c r="C23" t="str">
+        <v>€ 29,50</v>
+      </c>
+      <c r="D23" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>Ede</v>
+      </c>
+      <c r="B24" t="str">
+        <v>NS Ede - Wageningen (Bij bussen)</v>
+      </c>
+      <c r="C24" t="str">
+        <v>€ 27,00</v>
+      </c>
+      <c r="D24" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>Geldermalsen</v>
+      </c>
+      <c r="B25" t="str">
+        <v>NS station (P + R - Deilzeide)</v>
+      </c>
+      <c r="C25" t="str">
+        <v>€ 32,00</v>
+      </c>
+      <c r="D25" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>Groesbeek</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Bushalte gemeentehuis</v>
+      </c>
+      <c r="C26" t="str">
+        <v>€ 27,50</v>
+      </c>
+      <c r="D26" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>Hengelo GLD</v>
+      </c>
+      <c r="B27" t="str">
+        <v>Vordenseweg (THV Boerderij Groot-Roessink)</v>
+      </c>
+      <c r="C27" t="str">
+        <v>€ 30,50</v>
+      </c>
+      <c r="D27" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>Nijkerk</v>
+      </c>
+      <c r="B28" t="str">
+        <v>McDonalds</v>
+      </c>
+      <c r="C28" t="str">
+        <v>€ 31,50</v>
+      </c>
+      <c r="D28" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>Nijmegen</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Centraal Station (t.h.v. Van Bruggen Adviesgroep)</v>
+      </c>
+      <c r="C29" t="str">
+        <v>€ 26,00</v>
+      </c>
+      <c r="D29" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>Nunspeet</v>
+      </c>
+      <c r="B30" t="str">
+        <v>Nunspeet Tranferium</v>
+      </c>
+      <c r="C30" t="str">
+        <v>€ 33,00</v>
+      </c>
+      <c r="D30" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>Otterlo</v>
+      </c>
+      <c r="B31" t="str">
+        <v>TinQ Tankstation</v>
+      </c>
+      <c r="C31" t="str">
+        <v>€ 27,00</v>
+      </c>
+      <c r="D31" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>Vaassen</v>
+      </c>
+      <c r="B32" t="str">
+        <v>BP de Vink</v>
+      </c>
+      <c r="C32" t="str">
+        <v>€ 30,50</v>
+      </c>
+      <c r="D32" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>Amersfoort</v>
+      </c>
+      <c r="B33" t="str">
+        <v>Shell (hogeweg)</v>
+      </c>
+      <c r="C33" t="str">
+        <v>€ 32,00</v>
+      </c>
+      <c r="D33" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>Utrecht</v>
+      </c>
+      <c r="B34" t="str">
+        <v>Internationale busstop t.h.v. NH Hotel</v>
+      </c>
+      <c r="C34" t="str">
+        <v>€ 33,50</v>
+      </c>
+      <c r="D34" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>Woerden</v>
+      </c>
+      <c r="B35" t="str">
+        <v>NS station (Zuid)</v>
+      </c>
+      <c r="C35" t="str">
+        <v>€ 35,50</v>
+      </c>
+      <c r="D35" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>Aalsmeer</v>
+      </c>
+      <c r="B36" t="str">
+        <v>Hortensiaplein (bushalte)</v>
+      </c>
+      <c r="C36" t="str">
+        <v>€ 39,00</v>
+      </c>
+      <c r="D36" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>Alkmaar</v>
+      </c>
+      <c r="B37" t="str">
+        <v>NS Noord</v>
+      </c>
+      <c r="C37" t="str">
+        <v>€ 42,00</v>
+      </c>
+      <c r="D37" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>Amstelveen</v>
+      </c>
+      <c r="B38" t="str">
+        <v>Busstation Amstelveen</v>
+      </c>
+      <c r="C38" t="str">
+        <v>€ 38,50</v>
+      </c>
+      <c r="D38" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>Amsterdam</v>
+      </c>
+      <c r="B39" t="str">
+        <v>NS Zuid Bus stop (t.h.v. WTC)</v>
+      </c>
+      <c r="C39" t="str">
+        <v>€ 38,50</v>
+      </c>
+      <c r="D39" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>Amsterdam</v>
+      </c>
+      <c r="B40" t="str">
+        <v>NS K+R Sloterdijk (bovenop de brug)</v>
+      </c>
+      <c r="C40" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D40" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>Amsterdam</v>
+      </c>
+      <c r="B41" t="str">
+        <v>NS Amstel (next to tramstation)</v>
+      </c>
+      <c r="C41" t="str">
+        <v>€ 38,00</v>
+      </c>
+      <c r="D41" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>Beverwijk</v>
+      </c>
+      <c r="B42" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C42" t="str">
+        <v>€ 41,00</v>
+      </c>
+      <c r="D42" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>Grootebroek</v>
+      </c>
+      <c r="B43" t="str">
+        <v>Parkeerplaats Sportcomplex De Kloet</v>
+      </c>
+      <c r="C43" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D43" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>Haarlem</v>
+      </c>
+      <c r="B44" t="str">
+        <v>NS Centraal (busplaats)</v>
+      </c>
+      <c r="C44" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D44" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>Haarlem</v>
+      </c>
+      <c r="B45" t="str">
+        <v>P+R Haarlem Spaarnwoude</v>
+      </c>
+      <c r="C45" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D45" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>Hillegom</v>
+      </c>
+      <c r="B46" t="str">
+        <v>Bushalte Centrum</v>
+      </c>
+      <c r="C46" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D46" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>Hilversum</v>
+      </c>
+      <c r="B47" t="str">
+        <v>NS Sportpark (ESSO)</v>
+      </c>
+      <c r="C47" t="str">
+        <v>€ 34,50</v>
+      </c>
+      <c r="D47" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>Hoofddorp</v>
+      </c>
+      <c r="B48" t="str">
+        <v>Bushaltes</v>
+      </c>
+      <c r="C48" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D48" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>Hoofddorp</v>
+      </c>
+      <c r="B49" t="str">
+        <v>Bastion Hotel</v>
+      </c>
+      <c r="C49" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D49" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>Hoorn</v>
+      </c>
+      <c r="B50" t="str">
+        <v>Busplaatsen</v>
+      </c>
+      <c r="C50" t="str">
+        <v>€ 42,00</v>
+      </c>
+      <c r="D50" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>IJmuiden</v>
+      </c>
+      <c r="B51" t="str">
+        <v>IJmuiden velserduinplein</v>
+      </c>
+      <c r="C51" t="str">
+        <v>€ 41,00</v>
+      </c>
+      <c r="D51" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>Purmerend</v>
+      </c>
+      <c r="B52" t="str">
+        <v>Bushalte Canberrastraat (Weidevenne, Australiëlaan)</v>
+      </c>
+      <c r="C52" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D52" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>Schagen</v>
+      </c>
+      <c r="B53" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C53" t="str">
+        <v>€ 43,00</v>
+      </c>
+      <c r="D53" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>Schiphol</v>
+      </c>
+      <c r="B54" t="str">
+        <v>AMS Schiphol (Aankomstpassage tourbushaltes)</v>
+      </c>
+      <c r="C54" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D54" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>Schiphol</v>
+      </c>
+      <c r="B55" t="str">
+        <v>AMS Schiphol (Aankomstpassage tourbushaltes)</v>
+      </c>
+      <c r="C55" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D55" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>Velsen-Zuid</v>
+      </c>
+      <c r="B56" t="str">
+        <v>Stadion Telstar 1963 (Parkeerplaats)</v>
+      </c>
+      <c r="C56" t="str">
+        <v>€ 41,00</v>
+      </c>
+      <c r="D56" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>Alphen aan den Rijn</v>
+      </c>
+      <c r="B57" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C57" t="str">
+        <v>€ 38,50</v>
+      </c>
+      <c r="D57" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>Delft</v>
+      </c>
+      <c r="B58" t="str">
+        <v>Hampshire hotel Delft Centre</v>
+      </c>
+      <c r="C58" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D58" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>Den Haag</v>
+      </c>
+      <c r="B59" t="str">
+        <v>Busplaatsen thv. Academie van Beeldende Kunsten</v>
+      </c>
+      <c r="C59" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D59" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>Dordrecht</v>
+      </c>
+      <c r="B60" t="str">
+        <v>NS Centraal (Voorzijde - bij de stadsbussen)</v>
+      </c>
+      <c r="C60" t="str">
+        <v>€ 38,50</v>
+      </c>
+      <c r="D60" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>Gorinchem</v>
+      </c>
+      <c r="B61" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C61" t="str">
+        <v>€ 35,00</v>
+      </c>
+      <c r="D61" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>Gouda</v>
+      </c>
+      <c r="B62" t="str">
+        <v>Station (Achterzijde t.h.v. Cinema Gouda)</v>
+      </c>
+      <c r="C62" t="str">
+        <v>€ 38,00</v>
+      </c>
+      <c r="D62" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>Hillegom</v>
+      </c>
+      <c r="B63" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C63" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D63" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>Katwijk</v>
+      </c>
+      <c r="B64" t="str">
+        <v>Parkeerplaats vv Katwijk</v>
+      </c>
+      <c r="C64" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D64" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>Krimpen aan de Lek</v>
+      </c>
+      <c r="B65" t="str">
+        <v>Bushalte De Viersprong (N210, rotonde)</v>
+      </c>
+      <c r="C65" t="str">
+        <v>€ 39,00</v>
+      </c>
+      <c r="D65" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>Krimpen aan den IJssel</v>
+      </c>
+      <c r="B66" t="str">
+        <v>Zwembad De Lansingh</v>
+      </c>
+      <c r="C66" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D66" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>Leiden</v>
+      </c>
+      <c r="B67" t="str">
+        <v>NS Lammenschans</v>
+      </c>
+      <c r="C67" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D67" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>Nootdorp</v>
+      </c>
+      <c r="B68" t="str">
+        <v>Metrostation Nootdorp P+R (Industriezijde)</v>
+      </c>
+      <c r="C68" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D68" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>Rotterdam</v>
+      </c>
+      <c r="B69" t="str">
+        <v>NS Centraal (Kiss &amp; Ride) - Conradstraat</v>
+      </c>
+      <c r="C69" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D69" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>Rotterdam</v>
+      </c>
+      <c r="B70" t="str">
+        <v>Metrostation Slinge (bushalte aan Zuiderparkweg)</v>
+      </c>
+      <c r="C70" t="str">
+        <v>€ 40,00</v>
+      </c>
+      <c r="D70" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>Schiedam</v>
+      </c>
+      <c r="B71" t="str">
+        <v>Sporthal Margriet</v>
+      </c>
+      <c r="C71" t="str">
+        <v>€ 41,00</v>
+      </c>
+      <c r="D71" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>Spijkenisse</v>
+      </c>
+      <c r="B72" t="str">
+        <v>Kinepolis</v>
+      </c>
+      <c r="C72" t="str">
+        <v>€ 40,50</v>
+      </c>
+      <c r="D72" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>Zoetermeer</v>
+      </c>
+      <c r="B73" t="str">
+        <v>Centrum West Bushalte</v>
+      </c>
+      <c r="C73" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D73" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>Bergeijk</v>
+      </c>
+      <c r="B74" t="str">
+        <v>TotalEnergies (Parkeerplaats)</v>
+      </c>
+      <c r="C74" t="str">
+        <v>€ 39,00</v>
+      </c>
+      <c r="D74" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>Breda</v>
+      </c>
+      <c r="B75" t="str">
+        <v>NS station - Stationslaan - (Belcrum zijde)</v>
+      </c>
+      <c r="C75" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D75" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>Breda</v>
+      </c>
+      <c r="B76" t="str">
+        <v>Velderhof Meubelwinkel</v>
+      </c>
+      <c r="C76" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D76" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>Cuijk</v>
+      </c>
+      <c r="B77" t="str">
+        <v>McDonalds</v>
+      </c>
+      <c r="C77" t="str">
+        <v>€ 29,00</v>
+      </c>
+      <c r="D77" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>Den Bosch</v>
+      </c>
+      <c r="B78" t="str">
+        <v>Den Bosch Voorzijde CS (t.h.v. Gouden Draak)</v>
+      </c>
+      <c r="C78" t="str">
+        <v>€ 33,50</v>
+      </c>
+      <c r="D78" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>Eindhoven</v>
+      </c>
+      <c r="B79" t="str">
+        <v>NS station (flixbushalte thv Flying Pins)</v>
+      </c>
+      <c r="C79" t="str">
+        <v>€ 35,50</v>
+      </c>
+      <c r="D79" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>Heesch</v>
+      </c>
+      <c r="B80" t="str">
+        <v>McDonalds</v>
+      </c>
+      <c r="C80" t="str">
+        <v>€ 30,50</v>
+      </c>
+      <c r="D80" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>Helmond</v>
+      </c>
+      <c r="B81" t="str">
+        <v>NS Centraal (Stationsplein)</v>
+      </c>
+      <c r="C81" t="str">
+        <v>€ 35,50</v>
+      </c>
+      <c r="D81" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>Roosendaal</v>
+      </c>
+      <c r="B82" t="str">
+        <v>De Stok (Parkeerplaats)</v>
+      </c>
+      <c r="C82" t="str">
+        <v>€ 41,50</v>
+      </c>
+      <c r="D82" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>Tilburg</v>
+      </c>
+      <c r="B83" t="str">
+        <v>NS Centraal - Bushalte (Achterzijde)</v>
+      </c>
+      <c r="C83" t="str">
+        <v>€ 36,00</v>
+      </c>
+      <c r="D83" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>Veldhoven</v>
+      </c>
+      <c r="B84" t="str">
+        <v>Plein D'ekker</v>
+      </c>
+      <c r="C84" t="str">
+        <v>€ 37,00</v>
+      </c>
+      <c r="D84" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>Waspik</v>
+      </c>
+      <c r="B85" t="str">
+        <v>Parkeerplaats thv Aldi</v>
+      </c>
+      <c r="C85" t="str">
+        <v>€ 37,00</v>
+      </c>
+      <c r="D85" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>Heerlen</v>
+      </c>
+      <c r="B86" t="str">
+        <v>NS Centraal (bushaltes)</v>
+      </c>
+      <c r="C86" t="str">
+        <v>€ 43,00</v>
+      </c>
+      <c r="D86" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>Kerkrade</v>
+      </c>
+      <c r="B87" t="str">
+        <v>NS Centrum</v>
+      </c>
+      <c r="C87" t="str">
+        <v>€ 43,50</v>
+      </c>
+      <c r="D87" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>Maastricht</v>
+      </c>
+      <c r="B88" t="str">
+        <v>parkeerplaats Geusselt Maastricht</v>
+      </c>
+      <c r="C88" t="str">
+        <v>€ 43,00</v>
+      </c>
+      <c r="D88" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>Roermond</v>
+      </c>
+      <c r="B89" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C89" t="str">
+        <v>€ 39,50</v>
+      </c>
+      <c r="D89" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>Venlo</v>
+      </c>
+      <c r="B90" t="str">
+        <v>NS station</v>
+      </c>
+      <c r="C90" t="str">
+        <v>€ 36,50</v>
+      </c>
+      <c r="D90" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>Well</v>
+      </c>
+      <c r="B91" t="str">
+        <v>BP Tankstation Moleneind</v>
+      </c>
+      <c r="C91" t="str">
+        <v>€ 33,50</v>
+      </c>
+      <c r="D91" t="str">
+        <v>1 oktober</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
         <v>Wellerlooi</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B92" t="str">
         <v>Bushalte Catharinastraat</v>
       </c>
-      <c r="C8" t="str">
+      <c r="C92" t="str">
         <v>€ 34,00</v>
       </c>
-      <c r="D8" t="str">
+      <c r="D92" t="str">
         <v>1 oktober</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D92"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added data retrieval from api request to eleven travel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gijsvandenbeuken/Desktop/pb-scraper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBC96A4-8C73-8A45-87BE-1AF778AA7BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF621076-8638-6549-A450-0B7FCD560628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <t>NS Centraal (Flixbus halte)</t>
   </si>
   <si>
-    <t>€ 44,00</t>
+    <t>44,00</t>
   </si>
   <si>
     <t>1 oktober</t>
@@ -55,7 +55,7 @@
     <t>NS station (Bushaltes)</t>
   </si>
   <si>
-    <t>€ 45,00</t>
+    <t>45,00</t>
   </si>
   <si>
     <t>Friesland</t>
@@ -73,7 +73,7 @@
     <t>McDonalds Heerenveen</t>
   </si>
   <si>
-    <t>€ 41,50</t>
+    <t>41,50</t>
   </si>
   <si>
     <t>Leeuwarden</t>
@@ -82,7 +82,7 @@
     <t>NS station</t>
   </si>
   <si>
-    <t>€ 43,50</t>
+    <t>43,50</t>
   </si>
   <si>
     <t>uitstapbushalte busstation, stationsplein (Perron K)</t>
@@ -94,7 +94,7 @@
     <t>Assen</t>
   </si>
   <si>
-    <t>€ 42,50</t>
+    <t>42,50</t>
   </si>
   <si>
     <t>Emmen</t>
@@ -103,7 +103,7 @@
     <t>Meppel</t>
   </si>
   <si>
-    <t>€ 38,00</t>
+    <t>38,00</t>
   </si>
   <si>
     <t>Overijssel</t>
@@ -115,7 +115,7 @@
     <t>NS centraal (achterzijde parkeerplaats)</t>
   </si>
   <si>
-    <t>€ 36,50</t>
+    <t>36,50</t>
   </si>
   <si>
     <t>Tourbushalte (thv ingang java toren)</t>
@@ -127,7 +127,7 @@
     <t>Bushalte Zwiersstraat thv Skatebaan</t>
   </si>
   <si>
-    <t>€ 38,50</t>
+    <t>38,50</t>
   </si>
   <si>
     <t>Enschede</t>
@@ -139,13 +139,13 @@
     <t>Hardenberg</t>
   </si>
   <si>
-    <t>€ 39,50</t>
+    <t>39,50</t>
   </si>
   <si>
     <t>Hengelo</t>
   </si>
   <si>
-    <t>€ 37,00</t>
+    <t>37,00</t>
   </si>
   <si>
     <t>Schouwburg Hengelo</t>
@@ -157,7 +157,7 @@
     <t>P+R Rijssen (Achterzijde NS Station Rijssen)</t>
   </si>
   <si>
-    <t>€ 34,50</t>
+    <t>34,50</t>
   </si>
   <si>
     <t>Zwolle</t>
@@ -166,7 +166,7 @@
     <t>NS Centraal (achterzijde)</t>
   </si>
   <si>
-    <t>€ 34,00</t>
+    <t>34,00</t>
   </si>
   <si>
     <t>Flevoland</t>
@@ -187,7 +187,7 @@
     <t>Restaurant Orange (achterzijde)</t>
   </si>
   <si>
-    <t>€ 28,50</t>
+    <t>28,50</t>
   </si>
   <si>
     <t>Barneveld</t>
@@ -196,7 +196,7 @@
     <t>NS Centrum</t>
   </si>
   <si>
-    <t>€ 29,50</t>
+    <t>29,50</t>
   </si>
   <si>
     <t>Ede</t>
@@ -205,7 +205,7 @@
     <t>NS Ede - Wageningen (Bij bussen)</t>
   </si>
   <si>
-    <t>€ 27,00</t>
+    <t>27,00</t>
   </si>
   <si>
     <t>Geldermalsen</t>
@@ -214,7 +214,7 @@
     <t>NS station (P + R - Deilzeide)</t>
   </si>
   <si>
-    <t>€ 32,00</t>
+    <t>32,00</t>
   </si>
   <si>
     <t>Groesbeek</t>
@@ -223,7 +223,7 @@
     <t>Bushalte gemeentehuis</t>
   </si>
   <si>
-    <t>€ 27,50</t>
+    <t>27,50</t>
   </si>
   <si>
     <t>Hengelo GLD</t>
@@ -232,7 +232,7 @@
     <t>Vordenseweg (THV Boerderij Groot-Roessink)</t>
   </si>
   <si>
-    <t>€ 30,50</t>
+    <t>30,50</t>
   </si>
   <si>
     <t>Nijkerk</t>
@@ -241,7 +241,7 @@
     <t>McDonalds</t>
   </si>
   <si>
-    <t>€ 31,50</t>
+    <t>31,50</t>
   </si>
   <si>
     <t>Nijmegen</t>
@@ -250,7 +250,7 @@
     <t>Centraal Station (t.h.v. Van Bruggen Adviesgroep)</t>
   </si>
   <si>
-    <t>€ 26,00</t>
+    <t>26,00</t>
   </si>
   <si>
     <t>Nunspeet</t>
@@ -259,7 +259,7 @@
     <t>Nunspeet Tranferium</t>
   </si>
   <si>
-    <t>€ 33,00</t>
+    <t>33,00</t>
   </si>
   <si>
     <t>Otterlo</t>
@@ -286,7 +286,7 @@
     <t>Internationale busstop t.h.v. NH Hotel</t>
   </si>
   <si>
-    <t>€ 33,50</t>
+    <t>33,50</t>
   </si>
   <si>
     <t>Woerden</t>
@@ -295,7 +295,7 @@
     <t>NS station (Zuid)</t>
   </si>
   <si>
-    <t>€ 35,50</t>
+    <t>35,50</t>
   </si>
   <si>
     <t>Noord-Holland</t>
@@ -307,7 +307,7 @@
     <t>Hortensiaplein (bushalte)</t>
   </si>
   <si>
-    <t>€ 39,00</t>
+    <t>39,00</t>
   </si>
   <si>
     <t>Alkmaar</t>
@@ -316,7 +316,7 @@
     <t>NS Noord</t>
   </si>
   <si>
-    <t>€ 42,00</t>
+    <t>42,00</t>
   </si>
   <si>
     <t>Amstelveen</t>
@@ -340,7 +340,7 @@
     <t>Beverwijk</t>
   </si>
   <si>
-    <t>€ 41,00</t>
+    <t>41,00</t>
   </si>
   <si>
     <t>Grootebroek</t>
@@ -349,7 +349,7 @@
     <t>Parkeerplaats Sportcomplex De Kloet</t>
   </si>
   <si>
-    <t>€ 40,50</t>
+    <t>40,50</t>
   </si>
   <si>
     <t>Haarlem</t>
@@ -361,7 +361,7 @@
     <t>P+R Haarlem Spaarnwoude</t>
   </si>
   <si>
-    <t>€ 40,00</t>
+    <t>40,00</t>
   </si>
   <si>
     <t>Hillegom</t>
@@ -406,7 +406,7 @@
     <t>Schagen</t>
   </si>
   <si>
-    <t>€ 43,00</t>
+    <t>43,00</t>
   </si>
   <si>
     <t>Schiphol</t>
@@ -448,7 +448,7 @@
     <t>Gorinchem</t>
   </si>
   <si>
-    <t>€ 35,00</t>
+    <t>35,00</t>
   </si>
   <si>
     <t>Gouda</t>
@@ -535,7 +535,7 @@
     <t>Cuijk</t>
   </si>
   <si>
-    <t>€ 29,00</t>
+    <t>29,00</t>
   </si>
   <si>
     <t>Den Bosch</t>
@@ -571,7 +571,7 @@
     <t>NS Centraal - Bushalte (Achterzijde)</t>
   </si>
   <si>
-    <t>€ 36,00</t>
+    <t>36,00</t>
   </si>
   <si>
     <t>Veldhoven</t>
@@ -998,17 +998,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="65.5" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>